<commit_message>
Updated metrric 3 correlation
</commit_message>
<xml_diff>
--- a/Correlation/Metric 1,2 and 3 correlation.xlsx
+++ b/Correlation/Metric 1,2 and 3 correlation.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A076C9-149E-4A26-AC2F-162E9AF8FD0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1FCC3D-9916-410C-9D9D-857B78968F50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Project name</t>
   </si>
   <si>
-    <t>Mutation coverage</t>
-  </si>
-  <si>
     <t>confluence</t>
   </si>
   <si>
@@ -75,15 +72,9 @@
     <t>xhtml</t>
   </si>
   <si>
-    <t>average</t>
-  </si>
-  <si>
     <t>core</t>
   </si>
   <si>
-    <t>average between core and module</t>
-  </si>
-  <si>
     <t>Deltaspike 1.9</t>
   </si>
   <si>
@@ -102,9 +93,6 @@
     <t>Module</t>
   </si>
   <si>
-    <t>cdictrl</t>
-  </si>
-  <si>
     <t>module.proxy</t>
   </si>
   <si>
@@ -126,12 +114,6 @@
     <t>module.testcontrol</t>
   </si>
   <si>
-    <t>module average</t>
-  </si>
-  <si>
-    <t>core cdictrl module avg</t>
-  </si>
-  <si>
     <t>Statement Coverage</t>
   </si>
   <si>
@@ -139,13 +121,37 @@
   </si>
   <si>
     <t>Mutation Coverage</t>
+  </si>
+  <si>
+    <t>Project level</t>
+  </si>
+  <si>
+    <t>Project level mutaion coverage</t>
+  </si>
+  <si>
+    <t>killed mutants</t>
+  </si>
+  <si>
+    <t>total mutants</t>
+  </si>
+  <si>
+    <t>core.api</t>
+  </si>
+  <si>
+    <t>cdictrl.servlet</t>
+  </si>
+  <si>
+    <t>Project level coverage</t>
+  </si>
+  <si>
+    <t>Sum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +166,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="2">
@@ -202,7 +213,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -226,21 +237,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>349250</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8AD1788-60F2-48F9-AF44-BCD7F8E2FFDF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37653D17-0337-41CE-8651-8AA1E9AF999C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -256,7 +267,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1473200"/>
+          <a:off x="0" y="1454150"/>
           <a:ext cx="6096000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -268,23 +279,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66ABA579-D713-4C9C-BDDA-AAC5E26B33C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{840BAFB0-8012-4401-828B-0AC6EDC58E51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -300,7 +311,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6356350" y="1473200"/>
+          <a:off x="6102350" y="1397000"/>
           <a:ext cx="6096000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -576,101 +587,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="23.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="D2" s="3">
         <v>0.43</v>
       </c>
-      <c r="D2" s="3">
-        <v>0.49</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3">
         <v>0.9</v>
       </c>
+      <c r="C3" s="3">
+        <v>0.95</v>
+      </c>
       <c r="D3" s="3">
-        <v>0.95</v>
-      </c>
-      <c r="E3" s="3">
         <v>0.91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3">
         <v>0.85</v>
       </c>
+      <c r="C4" s="3">
+        <v>0.87</v>
+      </c>
       <c r="D4" s="3">
-        <v>0.87</v>
-      </c>
-      <c r="E4" s="3">
         <v>0.83</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3">
         <v>0.24</v>
       </c>
+      <c r="C5" s="3">
+        <v>0.21</v>
+      </c>
       <c r="D5" s="3">
         <v>0.21</v>
       </c>
-      <c r="E5" s="3">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3">
-        <v>0.6</v>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.8</v>
       </c>
       <c r="D6" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="E6" s="3">
         <v>0.66</v>
       </c>
     </row>
@@ -683,142 +694,193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CA9789-C5F3-4D68-B78D-7009EDBBA9EB}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>421</v>
+      </c>
+      <c r="C2">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>490</v>
+      </c>
+      <c r="C3">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>141</v>
+      </c>
+      <c r="C4">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>642</v>
+      </c>
+      <c r="C5">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>190</v>
+      </c>
+      <c r="C6">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>148</v>
+      </c>
+      <c r="C7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>562</v>
+      </c>
+      <c r="C9">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>449</v>
+      </c>
+      <c r="C11">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>196</v>
+      </c>
+      <c r="C12">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>80</v>
+      </c>
+      <c r="C13">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <f>AVERAGE(B2:B13)</f>
-        <v>0.66999999999999993</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
+      <c r="B15">
+        <v>1628</v>
+      </c>
+      <c r="C15">
+        <v>3031</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B2:B15)</f>
+        <v>5019</v>
+      </c>
+      <c r="C17">
+        <f>SUM(C2:C15)</f>
+        <v>8909</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B18">
-        <f>AVERAGE(B16,B14)</f>
-        <v>0.60499999999999998</v>
+        <f>B17/C17</f>
+        <v>0.56336289145807605</v>
       </c>
     </row>
   </sheetData>
@@ -829,114 +891,135 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E215B2-E30C-4D65-820A-5D21B7ED8C1D}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="4">
+        <v>182</v>
+      </c>
+      <c r="C2">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>129</v>
+      </c>
+      <c r="C4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B6">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B4">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B5">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B9">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B6">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
       <c r="B10">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="4">
-        <f>AVERAGE(B4:B10)</f>
-        <v>0.45142857142857146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="4">
-        <f>AVERAGE(B11,B3,B2)</f>
-        <v>0.39714285714285708</v>
+        <v>125</v>
+      </c>
+      <c r="C10">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B2:B10)</f>
+        <v>518</v>
+      </c>
+      <c r="C11">
+        <f>SUM(C2:C10)</f>
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <f>B11/C11</f>
+        <v>0.23481414324569355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>